<commit_message>
Convert CSV to XLSX
Co-Authored-By: Jia Tee <73531134+JJTee@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/SocialMediaAnalysis/Output/outputData.xlsx
+++ b/SocialMediaAnalysis/Output/outputData.xlsx
@@ -20,15 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Very Positive</t>
+    <t>Very Negative</t>
   </si>
   <si>
     <t>Neutral</t>
   </si>
   <si>
-    <t>Very Negative</t>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Very Positive</t>
+  </si>
+  <si>
+    <t>Negative</t>
   </si>
 </sst>
 </file>
@@ -368,7 +374,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I7" sqref="I7 I7"/>
@@ -381,7 +387,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -389,7 +395,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -397,17 +403,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="B4" s="1">
-        <v>95</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B5" s="1">
-        <v>95</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix up sentiment analysis
</commit_message>
<xml_diff>
--- a/SocialMediaAnalysis/Output/outputData.xlsx
+++ b/SocialMediaAnalysis/Output/outputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoa-my.sharepoint.com/personal/xzha897_uoa_auckland_ac_nz/Documents/Documents/GitHub/social-media-analysis/SocialMediaAnalysis/Output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_2B61E46F7907AE2F867E1E1EAB4DF215343450AC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F761483-64E4-4825-8D7E-E08A241C3568}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_E04CA2714B07AE2F867E1E08936CEF231B2D10ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,18 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Very Negative</t>
-  </si>
-  <si>
-    <t>Neutral</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Positive</t>
-  </si>
-  <si>
-    <t>Very Positive</t>
   </si>
   <si>
     <t>Negative</t>
@@ -70,7 +61,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -374,11 +365,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9 D9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -387,7 +376,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -395,36 +384,12 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="B3" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="1">
-        <v>61</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>